<commit_message>
made an entrypoint of the application
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -1157,7 +1157,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1183,70 +1183,138 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>1978</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>1990</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>Present</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>2024-05-16 00:00:33</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>2089</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>Absent</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1978</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-05-16 12:38:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2089</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-05-16 12:38:08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the functionality to mearge the excel sheets into one
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12570" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12570" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="2024-05-15" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="2024-05-16" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-05-15" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2024-05-16" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2024-05-26" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Consolidated" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -36,7 +37,15 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FF3F3F76"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -51,29 +60,14 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -83,37 +77,6 @@
       <color rgb="FF800080"/>
       <sz val="11"/>
       <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -127,9 +90,17 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -141,15 +112,25 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -164,17 +145,37 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,187 +191,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,17 +400,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -429,46 +426,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,6 +465,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -507,148 +508,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="9" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1047,14 +1048,100 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Roll No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Attendance</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>1978</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>2024-05-15 23:58:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>2089</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1065,23 +1152,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Roll No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Attendance</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>1978</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>1978</t>
+          <t>1990</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -1098,49 +1214,32 @@
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>1990</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Absent</t>
+          <t>Present</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>2024-05-16 00:00:33</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2089</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Present</t>
+          <t>Absent</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>2024-05-15 23:58:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>2089</t>
-        </is>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -1157,7 +1256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1229,7 +1328,7 @@
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>2024-05-16 00:00:33</t>
+          <t>2024-05-26 02:29:26</t>
         </is>
       </c>
     </row>
@@ -1250,73 +1349,132 @@
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1978</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1990</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Absent</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2010</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>roll_no</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1978</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Present</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2024-05-16 12:38:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2089</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Present</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2024-05-16 12:38:08</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2089</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>